<commit_message>
correção de erros inventario
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -504,7 +504,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -533,6 +533,74 @@
           <t>valor</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>tipo</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>13/07/2025</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Saldo inicial do dia</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>entrada</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>13/07/2025</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">açogue </t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>-256.73</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>saida</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>13/07/2025</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Mercado</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>-238.73</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>saida</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
processo de bugfix missmatch column
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -463,7 +463,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>lucro</t>
+          <t>valor_venda</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>venda_id</t>
         </is>
       </c>
     </row>
@@ -504,7 +509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +525,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>categoria</t>
+          <t>tipo</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -531,11 +536,6 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>valor</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>tipo</t>
         </is>
       </c>
     </row>
@@ -545,7 +545,11 @@
           <t>13/07/2025</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>entrada</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Saldo inicial do dia</t>
@@ -553,11 +557,6 @@
       </c>
       <c r="D2" t="n">
         <v>0</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>entrada</t>
-        </is>
       </c>
     </row>
     <row r="3">
@@ -566,7 +565,11 @@
           <t>13/07/2025</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>saida</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
           <t xml:space="preserve">açogue </t>
@@ -574,11 +577,6 @@
       </c>
       <c r="D3" t="n">
         <v>-256.73</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>saida</t>
-        </is>
       </c>
     </row>
     <row r="4">
@@ -587,7 +585,11 @@
           <t>13/07/2025</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>saida</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>Mercado</t>
@@ -595,11 +597,6 @@
       </c>
       <c r="D4" t="n">
         <v>-238.73</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>saida</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>